<commit_message>
Add CP, ABS, AM groups in down tab and code notes
</commit_message>
<xml_diff>
--- a/Fiche_Exemple.xlsx
+++ b/Fiche_Exemple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur\Desktop\BOULOT\fiche de paie\Fiche_de_Paye\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EF1C98-0856-42E6-B9CA-83ABB85F00DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B442608-9F4C-42E7-BDF6-1737E2C7685B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4044450-EC2F-40B3-BDF9-568C0D9FF30A}"/>
   </bookViews>
@@ -132,9 +132,6 @@
     <t>Nb. Tickets restaurant :</t>
   </si>
   <si>
-    <t>Hres jour férié travaillé :</t>
-  </si>
-  <si>
     <t>AT :</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>Total :</t>
+  </si>
+  <si>
+    <t>Hres jour férié travaillé : 0</t>
   </si>
 </sst>
 </file>
@@ -631,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="46" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -731,144 +731,144 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -892,6 +892,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1236,10 +1250,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AB34"/>
+  <dimension ref="A2:AB37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13:AB13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="97" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1275,732 +1289,732 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
-      <c r="R2" s="74"/>
-      <c r="S2" s="74"/>
-      <c r="T2" s="74"/>
-      <c r="U2" s="74"/>
-      <c r="W2" s="84" t="s">
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="W2" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="39"/>
-      <c r="Z2" s="39"/>
+      <c r="X2" s="84"/>
+      <c r="Y2" s="84"/>
+      <c r="Z2" s="84"/>
       <c r="AA2" s="85"/>
       <c r="AB2" s="86"/>
     </row>
     <row r="3" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="74"/>
-      <c r="R3" s="74"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="74"/>
-      <c r="U3" s="74"/>
-      <c r="W3" s="81" t="s">
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="73"/>
+      <c r="W3" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="X3" s="82"/>
-      <c r="Y3" s="82"/>
-      <c r="Z3" s="82"/>
-      <c r="AA3" s="82"/>
-      <c r="AB3" s="83"/>
+      <c r="X3" s="81"/>
+      <c r="Y3" s="81"/>
+      <c r="Z3" s="81"/>
+      <c r="AA3" s="81"/>
+      <c r="AB3" s="82"/>
     </row>
     <row r="4" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74"/>
-      <c r="U4" s="74"/>
-      <c r="W4" s="78" t="s">
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="73"/>
+      <c r="W4" s="77" t="s">
         <v>23</v>
       </c>
       <c r="X4" s="38"/>
       <c r="Y4" s="38"/>
       <c r="Z4" s="38"/>
-      <c r="AA4" s="79" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB4" s="80"/>
+      <c r="AA4" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB4" s="79"/>
     </row>
     <row r="5" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="74"/>
-      <c r="T5" s="74"/>
-      <c r="U5" s="74"/>
-      <c r="W5" s="81" t="s">
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="73"/>
+      <c r="W5" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="82"/>
-      <c r="Z5" s="82"/>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="83"/>
+      <c r="X5" s="81"/>
+      <c r="Y5" s="81"/>
+      <c r="Z5" s="81"/>
+      <c r="AA5" s="81"/>
+      <c r="AB5" s="82"/>
     </row>
     <row r="6" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="74"/>
-      <c r="R6" s="74"/>
-      <c r="S6" s="74"/>
-      <c r="T6" s="74"/>
-      <c r="U6" s="74"/>
-      <c r="W6" s="78" t="s">
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="73"/>
+      <c r="S6" s="73"/>
+      <c r="T6" s="73"/>
+      <c r="U6" s="73"/>
+      <c r="W6" s="77" t="s">
         <v>19</v>
       </c>
       <c r="X6" s="38"/>
       <c r="Y6" s="38"/>
       <c r="Z6" s="38"/>
-      <c r="AA6" s="79"/>
-      <c r="AB6" s="80"/>
+      <c r="AA6" s="78"/>
+      <c r="AB6" s="79"/>
     </row>
     <row r="7" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="74"/>
-      <c r="T7" s="74"/>
-      <c r="U7" s="74"/>
-      <c r="W7" s="75" t="s">
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="73"/>
+      <c r="S7" s="73"/>
+      <c r="T7" s="73"/>
+      <c r="U7" s="73"/>
+      <c r="W7" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="X7" s="76"/>
-      <c r="Y7" s="76"/>
-      <c r="Z7" s="76"/>
-      <c r="AA7" s="76"/>
-      <c r="AB7" s="77"/>
+      <c r="X7" s="75"/>
+      <c r="Y7" s="75"/>
+      <c r="Z7" s="75"/>
+      <c r="AA7" s="75"/>
+      <c r="AB7" s="76"/>
     </row>
     <row r="9" spans="1:28" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="41"/>
-      <c r="T9" s="41"/>
-      <c r="U9" s="41"/>
-      <c r="V9" s="41"/>
-      <c r="W9" s="41"/>
-      <c r="X9" s="41"/>
-      <c r="Y9" s="41"/>
-      <c r="Z9" s="41"/>
-      <c r="AA9" s="41"/>
-      <c r="AB9" s="42"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
+      <c r="V9" s="40"/>
+      <c r="W9" s="40"/>
+      <c r="X9" s="40"/>
+      <c r="Y9" s="40"/>
+      <c r="Z9" s="40"/>
+      <c r="AA9" s="40"/>
+      <c r="AB9" s="41"/>
     </row>
     <row r="10" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="51">
+      <c r="B10" s="50">
         <v>1</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="51">
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="50">
         <v>2</v>
       </c>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="51">
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="50">
         <v>3</v>
       </c>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="51">
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="52"/>
+      <c r="Q10" s="50">
         <v>4</v>
       </c>
-      <c r="R10" s="52"/>
-      <c r="S10" s="52"/>
-      <c r="T10" s="52"/>
-      <c r="U10" s="53"/>
-      <c r="V10" s="51">
+      <c r="R10" s="51"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="51"/>
+      <c r="U10" s="52"/>
+      <c r="V10" s="50">
         <v>5</v>
       </c>
-      <c r="W10" s="52"/>
-      <c r="X10" s="52"/>
-      <c r="Y10" s="52"/>
-      <c r="Z10" s="53"/>
-      <c r="AA10" s="56"/>
-      <c r="AB10" s="57"/>
+      <c r="W10" s="51"/>
+      <c r="X10" s="51"/>
+      <c r="Y10" s="51"/>
+      <c r="Z10" s="52"/>
+      <c r="AA10" s="55"/>
+      <c r="AB10" s="56"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="58"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="14"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="49"/>
+      <c r="G11" s="48"/>
       <c r="H11" s="18"/>
       <c r="I11" s="19"/>
       <c r="J11" s="20"/>
       <c r="K11" s="16"/>
-      <c r="L11" s="49"/>
+      <c r="L11" s="48"/>
       <c r="M11" s="24"/>
       <c r="N11" s="25"/>
       <c r="O11" s="26"/>
       <c r="P11" s="16"/>
-      <c r="Q11" s="49"/>
+      <c r="Q11" s="48"/>
       <c r="R11" s="18"/>
       <c r="S11" s="19"/>
       <c r="T11" s="20"/>
       <c r="U11" s="16"/>
-      <c r="V11" s="58"/>
+      <c r="V11" s="57"/>
       <c r="W11" s="18"/>
       <c r="X11" s="19"/>
       <c r="Y11" s="20"/>
       <c r="Z11" s="16"/>
-      <c r="AA11" s="43"/>
-      <c r="AB11" s="44"/>
+      <c r="AA11" s="42"/>
+      <c r="AB11" s="43"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A12" s="73"/>
-      <c r="B12" s="59"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="17"/>
-      <c r="G12" s="50"/>
+      <c r="G12" s="49"/>
       <c r="H12" s="21"/>
       <c r="I12" s="22"/>
       <c r="J12" s="23"/>
       <c r="K12" s="17"/>
-      <c r="L12" s="50"/>
+      <c r="L12" s="49"/>
       <c r="M12" s="27"/>
       <c r="N12" s="28"/>
       <c r="O12" s="29"/>
       <c r="P12" s="17"/>
-      <c r="Q12" s="50"/>
+      <c r="Q12" s="49"/>
       <c r="R12" s="21"/>
       <c r="S12" s="22"/>
       <c r="T12" s="23"/>
       <c r="U12" s="17"/>
-      <c r="V12" s="59"/>
+      <c r="V12" s="58"/>
       <c r="W12" s="21"/>
       <c r="X12" s="22"/>
       <c r="Y12" s="23"/>
       <c r="Z12" s="17"/>
-      <c r="AA12" s="43"/>
-      <c r="AB12" s="44"/>
+      <c r="AA12" s="42"/>
+      <c r="AB12" s="43"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="49"/>
+      <c r="B13" s="48"/>
       <c r="C13" s="18"/>
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
       <c r="F13" s="16"/>
-      <c r="G13" s="49"/>
+      <c r="G13" s="48"/>
       <c r="H13" s="18"/>
       <c r="I13" s="19"/>
       <c r="J13" s="20"/>
       <c r="K13" s="16"/>
-      <c r="L13" s="49"/>
+      <c r="L13" s="48"/>
       <c r="M13" s="18"/>
       <c r="N13" s="19"/>
       <c r="O13" s="20"/>
       <c r="P13" s="16"/>
-      <c r="Q13" s="49"/>
+      <c r="Q13" s="48"/>
       <c r="R13" s="18"/>
       <c r="S13" s="19"/>
       <c r="T13" s="20"/>
       <c r="U13" s="16"/>
-      <c r="V13" s="49"/>
+      <c r="V13" s="48"/>
       <c r="W13" s="18"/>
       <c r="X13" s="19"/>
       <c r="Y13" s="20"/>
       <c r="Z13" s="16"/>
-      <c r="AA13" s="67" t="s">
+      <c r="AA13" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="AB13" s="68"/>
+      <c r="AB13" s="67"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A14" s="73"/>
-      <c r="B14" s="50"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="21"/>
       <c r="D14" s="22"/>
       <c r="E14" s="23"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="50"/>
+      <c r="G14" s="49"/>
       <c r="H14" s="21"/>
       <c r="I14" s="22"/>
       <c r="J14" s="23"/>
       <c r="K14" s="17"/>
-      <c r="L14" s="50"/>
+      <c r="L14" s="49"/>
       <c r="M14" s="21"/>
       <c r="N14" s="22"/>
       <c r="O14" s="23"/>
       <c r="P14" s="17"/>
-      <c r="Q14" s="50"/>
+      <c r="Q14" s="49"/>
       <c r="R14" s="21"/>
       <c r="S14" s="22"/>
       <c r="T14" s="23"/>
       <c r="U14" s="17"/>
-      <c r="V14" s="50"/>
+      <c r="V14" s="49"/>
       <c r="W14" s="21"/>
       <c r="X14" s="22"/>
       <c r="Y14" s="23"/>
       <c r="Z14" s="17"/>
-      <c r="AA14" s="69" t="s">
+      <c r="AA14" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="AB14" s="68"/>
+      <c r="AB14" s="67"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A15" s="72" t="s">
+      <c r="A15" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="49"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="18"/>
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
       <c r="F15" s="16"/>
-      <c r="G15" s="49"/>
+      <c r="G15" s="48"/>
       <c r="H15" s="18"/>
       <c r="I15" s="19"/>
       <c r="J15" s="20"/>
       <c r="K15" s="16"/>
-      <c r="L15" s="49"/>
+      <c r="L15" s="48"/>
       <c r="M15" s="18"/>
       <c r="N15" s="19"/>
       <c r="O15" s="20"/>
       <c r="P15" s="16"/>
-      <c r="Q15" s="49"/>
+      <c r="Q15" s="48"/>
       <c r="R15" s="18"/>
       <c r="S15" s="19"/>
       <c r="T15" s="20"/>
       <c r="U15" s="16"/>
-      <c r="V15" s="49"/>
+      <c r="V15" s="48"/>
       <c r="W15" s="18"/>
       <c r="X15" s="19"/>
       <c r="Y15" s="20"/>
       <c r="Z15" s="16"/>
-      <c r="AA15" s="43"/>
-      <c r="AB15" s="44"/>
+      <c r="AA15" s="42"/>
+      <c r="AB15" s="43"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A16" s="73"/>
-      <c r="B16" s="50"/>
+      <c r="A16" s="72"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="21"/>
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="50"/>
+      <c r="G16" s="49"/>
       <c r="H16" s="21"/>
       <c r="I16" s="22"/>
       <c r="J16" s="23"/>
       <c r="K16" s="17"/>
-      <c r="L16" s="50"/>
+      <c r="L16" s="49"/>
       <c r="M16" s="21"/>
       <c r="N16" s="22"/>
       <c r="O16" s="23"/>
       <c r="P16" s="17"/>
-      <c r="Q16" s="50"/>
+      <c r="Q16" s="49"/>
       <c r="R16" s="21"/>
       <c r="S16" s="22"/>
       <c r="T16" s="23"/>
       <c r="U16" s="17"/>
-      <c r="V16" s="50"/>
+      <c r="V16" s="49"/>
       <c r="W16" s="21"/>
       <c r="X16" s="22"/>
       <c r="Y16" s="23"/>
       <c r="Z16" s="17"/>
-      <c r="AA16" s="67" t="s">
+      <c r="AA16" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="AB16" s="68"/>
+      <c r="AB16" s="67"/>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A17" s="72" t="s">
+      <c r="A17" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="49"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="18"/>
       <c r="D17" s="19"/>
       <c r="E17" s="20"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="49"/>
+      <c r="G17" s="48"/>
       <c r="H17" s="18"/>
       <c r="I17" s="19"/>
       <c r="J17" s="20"/>
       <c r="K17" s="16"/>
-      <c r="L17" s="49"/>
+      <c r="L17" s="48"/>
       <c r="M17" s="18"/>
       <c r="N17" s="19"/>
       <c r="O17" s="20"/>
       <c r="P17" s="16"/>
-      <c r="Q17" s="49"/>
+      <c r="Q17" s="48"/>
       <c r="R17" s="18"/>
       <c r="S17" s="19"/>
       <c r="T17" s="20"/>
       <c r="U17" s="16"/>
-      <c r="V17" s="49"/>
+      <c r="V17" s="48"/>
       <c r="W17" s="18"/>
       <c r="X17" s="19"/>
       <c r="Y17" s="20"/>
       <c r="Z17" s="16"/>
-      <c r="AA17" s="70" t="s">
+      <c r="AA17" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="AB17" s="68"/>
+      <c r="AB17" s="67"/>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A18" s="73"/>
-      <c r="B18" s="50"/>
+      <c r="A18" s="72"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="21"/>
       <c r="D18" s="22"/>
       <c r="E18" s="23"/>
       <c r="F18" s="17"/>
-      <c r="G18" s="50"/>
+      <c r="G18" s="49"/>
       <c r="H18" s="21"/>
       <c r="I18" s="22"/>
       <c r="J18" s="23"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="50"/>
+      <c r="L18" s="49"/>
       <c r="M18" s="21"/>
       <c r="N18" s="22"/>
       <c r="O18" s="23"/>
       <c r="P18" s="17"/>
-      <c r="Q18" s="50"/>
+      <c r="Q18" s="49"/>
       <c r="R18" s="21"/>
       <c r="S18" s="22"/>
       <c r="T18" s="23"/>
       <c r="U18" s="17"/>
-      <c r="V18" s="50"/>
+      <c r="V18" s="49"/>
       <c r="W18" s="21"/>
       <c r="X18" s="22"/>
       <c r="Y18" s="23"/>
       <c r="Z18" s="17"/>
-      <c r="AA18" s="43"/>
-      <c r="AB18" s="44"/>
+      <c r="AA18" s="42"/>
+      <c r="AB18" s="43"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A19" s="72" t="s">
+      <c r="A19" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="49"/>
+      <c r="B19" s="48"/>
       <c r="C19" s="18"/>
       <c r="D19" s="19"/>
       <c r="E19" s="20"/>
       <c r="F19" s="16"/>
-      <c r="G19" s="49"/>
+      <c r="G19" s="48"/>
       <c r="H19" s="18"/>
       <c r="I19" s="19"/>
       <c r="J19" s="20"/>
       <c r="K19" s="16"/>
-      <c r="L19" s="49"/>
+      <c r="L19" s="48"/>
       <c r="M19" s="18"/>
       <c r="N19" s="19"/>
       <c r="O19" s="20"/>
       <c r="P19" s="16"/>
-      <c r="Q19" s="49"/>
+      <c r="Q19" s="48"/>
       <c r="R19" s="18"/>
       <c r="S19" s="19"/>
       <c r="T19" s="20"/>
       <c r="U19" s="16"/>
-      <c r="V19" s="58"/>
+      <c r="V19" s="57"/>
       <c r="W19" s="15"/>
       <c r="X19" s="15"/>
       <c r="Y19" s="15"/>
       <c r="Z19" s="16"/>
-      <c r="AA19" s="43"/>
-      <c r="AB19" s="44"/>
+      <c r="AA19" s="42"/>
+      <c r="AB19" s="43"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A20" s="73"/>
-      <c r="B20" s="50"/>
+      <c r="A20" s="72"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="21"/>
       <c r="D20" s="22"/>
       <c r="E20" s="23"/>
       <c r="F20" s="17"/>
-      <c r="G20" s="50"/>
+      <c r="G20" s="49"/>
       <c r="H20" s="21"/>
       <c r="I20" s="22"/>
       <c r="J20" s="23"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="50"/>
+      <c r="L20" s="49"/>
       <c r="M20" s="21"/>
       <c r="N20" s="22"/>
       <c r="O20" s="23"/>
       <c r="P20" s="17"/>
-      <c r="Q20" s="50"/>
+      <c r="Q20" s="49"/>
       <c r="R20" s="21"/>
       <c r="S20" s="22"/>
       <c r="T20" s="23"/>
       <c r="U20" s="17"/>
-      <c r="V20" s="59"/>
+      <c r="V20" s="58"/>
       <c r="W20" s="21"/>
       <c r="X20" s="22"/>
       <c r="Y20" s="23"/>
       <c r="Z20" s="17"/>
-      <c r="AA20" s="45"/>
-      <c r="AB20" s="46"/>
+      <c r="AA20" s="44"/>
+      <c r="AB20" s="45"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A21" s="72" t="s">
+      <c r="A21" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="49"/>
+      <c r="B21" s="48"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="49"/>
+      <c r="G21" s="48"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="16"/>
-      <c r="L21" s="49"/>
+      <c r="L21" s="48"/>
       <c r="M21" s="15"/>
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
       <c r="P21" s="16"/>
-      <c r="Q21" s="49"/>
+      <c r="Q21" s="48"/>
       <c r="R21" s="15"/>
       <c r="S21" s="15"/>
       <c r="T21" s="15"/>
       <c r="U21" s="16"/>
-      <c r="V21" s="58"/>
+      <c r="V21" s="57"/>
       <c r="W21" s="15"/>
       <c r="X21" s="15"/>
       <c r="Y21" s="15"/>
       <c r="Z21" s="16"/>
-      <c r="AA21" s="47" t="s">
+      <c r="AA21" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="AB21" s="48"/>
+      <c r="AB21" s="47"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A22" s="73"/>
-      <c r="B22" s="50"/>
+      <c r="A22" s="72"/>
+      <c r="B22" s="49"/>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
       <c r="F22" s="17"/>
-      <c r="G22" s="50"/>
+      <c r="G22" s="49"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
       <c r="J22" s="23"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="50"/>
+      <c r="L22" s="49"/>
       <c r="M22" s="21"/>
       <c r="N22" s="22"/>
       <c r="O22" s="23"/>
       <c r="P22" s="17"/>
-      <c r="Q22" s="50"/>
+      <c r="Q22" s="49"/>
       <c r="R22" s="21"/>
       <c r="S22" s="22"/>
       <c r="T22" s="23"/>
       <c r="U22" s="17"/>
-      <c r="V22" s="59"/>
+      <c r="V22" s="58"/>
       <c r="W22" s="21"/>
       <c r="X22" s="22"/>
       <c r="Y22" s="23"/>
       <c r="Z22" s="17"/>
-      <c r="AA22" s="54"/>
-      <c r="AB22" s="55"/>
+      <c r="AA22" s="53"/>
+      <c r="AB22" s="54"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A23" s="72" t="s">
+      <c r="A23" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="49"/>
+      <c r="B23" s="48"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="16"/>
-      <c r="G23" s="49"/>
+      <c r="G23" s="48"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
       <c r="K23" s="16"/>
-      <c r="L23" s="49"/>
+      <c r="L23" s="48"/>
       <c r="M23" s="15"/>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
       <c r="P23" s="16"/>
-      <c r="Q23" s="49"/>
+      <c r="Q23" s="48"/>
       <c r="R23" s="15"/>
       <c r="S23" s="15"/>
       <c r="T23" s="15"/>
       <c r="U23" s="16"/>
-      <c r="V23" s="58"/>
+      <c r="V23" s="57"/>
       <c r="W23" s="15"/>
       <c r="X23" s="15"/>
       <c r="Y23" s="15"/>
       <c r="Z23" s="16"/>
-      <c r="AA23" s="63" t="s">
+      <c r="AA23" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="AB23" s="65" t="s">
+      <c r="AB23" s="64" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A24" s="73"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="72"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="21"/>
       <c r="D24" s="22"/>
       <c r="E24" s="23"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="50"/>
+      <c r="G24" s="49"/>
       <c r="H24" s="21"/>
       <c r="I24" s="22"/>
       <c r="J24" s="23"/>
       <c r="K24" s="17"/>
-      <c r="L24" s="50"/>
+      <c r="L24" s="49"/>
       <c r="M24" s="21"/>
       <c r="N24" s="22"/>
       <c r="O24" s="23"/>
       <c r="P24" s="17"/>
-      <c r="Q24" s="50"/>
+      <c r="Q24" s="49"/>
       <c r="R24" s="21"/>
       <c r="S24" s="22"/>
       <c r="T24" s="23"/>
       <c r="U24" s="17"/>
-      <c r="V24" s="59"/>
+      <c r="V24" s="58"/>
       <c r="W24" s="21"/>
       <c r="X24" s="22"/>
       <c r="Y24" s="23"/>
       <c r="Z24" s="17"/>
-      <c r="AA24" s="64"/>
-      <c r="AB24" s="66"/>
+      <c r="AA24" s="63"/>
+      <c r="AB24" s="65"/>
     </row>
     <row r="25" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="60">
+      <c r="B25" s="59">
         <v>1.1666666666666667</v>
       </c>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="60">
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="59">
         <v>1.4583333333333333</v>
       </c>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="62"/>
-      <c r="L25" s="60">
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="59">
         <v>1.1666666666666667</v>
       </c>
-      <c r="M25" s="61"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="61"/>
-      <c r="P25" s="62"/>
-      <c r="Q25" s="60">
+      <c r="M25" s="60"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="60"/>
+      <c r="P25" s="61"/>
+      <c r="Q25" s="59">
         <v>1.4583333333333333</v>
       </c>
-      <c r="R25" s="61"/>
-      <c r="S25" s="61"/>
-      <c r="T25" s="61"/>
-      <c r="U25" s="62"/>
-      <c r="V25" s="60">
+      <c r="R25" s="60"/>
+      <c r="S25" s="60"/>
+      <c r="T25" s="60"/>
+      <c r="U25" s="61"/>
+      <c r="V25" s="59">
         <v>1.1666666666666667</v>
       </c>
-      <c r="W25" s="61"/>
-      <c r="X25" s="61"/>
-      <c r="Y25" s="61"/>
-      <c r="Z25" s="62"/>
+      <c r="W25" s="60"/>
+      <c r="X25" s="60"/>
+      <c r="Y25" s="60"/>
+      <c r="Z25" s="61"/>
       <c r="AA25" s="2">
         <v>6.416666666666667</v>
       </c>
@@ -2051,10 +2065,10 @@
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="H27" s="39"/>
+      <c r="G27" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="84"/>
       <c r="I27" s="91"/>
       <c r="J27" s="91"/>
       <c r="K27" s="12" t="s">
@@ -2069,95 +2083,118 @@
       </c>
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
-      <c r="Q27" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="R27" s="39"/>
+      <c r="Q27" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="R27" s="84"/>
       <c r="S27" s="91"/>
       <c r="T27" s="91"/>
-      <c r="U27" s="39" t="s">
+      <c r="U27" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="V27" s="39"/>
-      <c r="W27" s="39"/>
-      <c r="X27" s="39"/>
-      <c r="Y27" s="39"/>
+      <c r="V27" s="84"/>
+      <c r="W27" s="84"/>
+      <c r="X27" s="84"/>
+      <c r="Y27" s="84"/>
       <c r="Z27" s="5">
         <v>0</v>
       </c>
-      <c r="AA27" s="39" t="s">
-        <v>30</v>
+      <c r="AA27" s="84" t="s">
+        <v>43</v>
       </c>
       <c r="AB27" s="90"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
-      <c r="B28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="U28" s="30"/>
-      <c r="V28" s="30"/>
-      <c r="W28" s="30"/>
-      <c r="X28" s="30"/>
-      <c r="Y28" s="30"/>
-      <c r="Z28" s="6"/>
-      <c r="AA28" s="30"/>
+      <c r="B28" s="93"/>
+      <c r="C28" s="94"/>
+      <c r="D28" s="93"/>
+      <c r="E28" s="95"/>
+      <c r="F28" s="95"/>
+      <c r="G28" s="96"/>
+      <c r="H28" s="96"/>
+      <c r="I28" s="97"/>
+      <c r="J28" s="97"/>
+      <c r="K28" s="98"/>
+      <c r="L28" s="93"/>
+      <c r="M28" s="95"/>
+      <c r="N28" s="93"/>
+      <c r="O28" s="95"/>
+      <c r="P28" s="95"/>
+      <c r="Q28" s="96"/>
+      <c r="R28" s="96"/>
+      <c r="S28" s="97"/>
+      <c r="T28" s="97"/>
+      <c r="U28" s="96"/>
+      <c r="V28" s="96"/>
+      <c r="W28" s="96"/>
+      <c r="X28" s="96"/>
+      <c r="Y28" s="96"/>
+      <c r="Z28" s="93"/>
+      <c r="AA28" s="96"/>
       <c r="AB28" s="35"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="37"/>
+      <c r="B29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="U29" s="30"/>
+      <c r="V29" s="30"/>
+      <c r="W29" s="30"/>
+      <c r="X29" s="30"/>
+      <c r="Y29" s="30"/>
+      <c r="Z29" s="6"/>
+      <c r="AA29" s="30"/>
+      <c r="AB29" s="35"/>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A30" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="34"/>
+      <c r="D30" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="34"/>
+      <c r="G30" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B29" t="s">
+      <c r="H30" s="38"/>
+      <c r="I30" s="92"/>
+      <c r="J30" s="92"/>
+      <c r="K30" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L30" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="32" t="s">
+      <c r="N30" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="34"/>
-      <c r="G29" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="H29" s="38"/>
-      <c r="I29" s="92"/>
-      <c r="J29" s="92"/>
-      <c r="K29" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="N29" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q29" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="R29" s="38"/>
-      <c r="S29" s="92"/>
-      <c r="T29" s="92"/>
-      <c r="U29" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA29" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB29" s="31"/>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A30" s="37"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="34"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="U30" s="30"/>
-      <c r="AA30" s="30"/>
-      <c r="AB30" s="8"/>
+      <c r="Q30" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="R30" s="38"/>
+      <c r="S30" s="92">
+        <v>0</v>
+      </c>
+      <c r="T30" s="92"/>
+      <c r="U30" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB30" s="31"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" s="37"/>
@@ -2172,114 +2209,159 @@
       <c r="AB31" s="8"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="37"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="34"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="U32" s="30"/>
+      <c r="AA32" s="30"/>
+      <c r="AB32" s="8"/>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A33" s="37"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="34"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="U33" s="30"/>
+      <c r="AA33" s="30"/>
+      <c r="AB33" s="8"/>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A34" s="37"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="34"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="U34" s="30"/>
+      <c r="AA34" s="30"/>
+      <c r="AB34" s="8"/>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A35" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="H35" s="38"/>
+      <c r="I35" s="92">
+        <v>0</v>
+      </c>
+      <c r="J35" s="92"/>
+      <c r="K35" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q35" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="R35" s="38"/>
+      <c r="S35" s="92">
+        <v>0</v>
+      </c>
+      <c r="T35" s="92"/>
+      <c r="U35" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="W35">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB35" s="31"/>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+      <c r="T36" s="10"/>
+      <c r="U36" s="10"/>
+      <c r="V36" s="10"/>
+      <c r="W36" s="10"/>
+      <c r="X36" s="10"/>
+      <c r="Y36" s="10"/>
+      <c r="Z36" s="10"/>
+      <c r="AA36" s="10"/>
+      <c r="AB36" s="11"/>
+    </row>
+    <row r="37" spans="1:28" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G32" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="H32" s="38"/>
-      <c r="I32" s="92"/>
-      <c r="J32" s="92"/>
-      <c r="K32" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="L32" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q32" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="R32" s="38"/>
-      <c r="S32" s="92"/>
-      <c r="T32" s="92"/>
-      <c r="U32" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA32" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB32" s="31"/>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="10"/>
-      <c r="T33" s="10"/>
-      <c r="U33" s="10"/>
-      <c r="V33" s="10"/>
-      <c r="W33" s="10"/>
-      <c r="X33" s="10"/>
-      <c r="Y33" s="10"/>
-      <c r="Z33" s="10"/>
-      <c r="AA33" s="10"/>
-      <c r="AB33" s="11"/>
-    </row>
-    <row r="34" spans="1:28" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="38" t="s">
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="M37" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="M34" s="38" t="s">
+      <c r="N37" s="38"/>
+      <c r="O37" s="38"/>
+      <c r="P37" s="38"/>
+      <c r="W37" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="N34" s="38"/>
-      <c r="O34" s="38"/>
-      <c r="P34" s="38"/>
-      <c r="W34" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="X34" s="38"/>
-      <c r="Y34" s="38"/>
-      <c r="Z34" s="38"/>
-      <c r="AA34" s="38"/>
-      <c r="AB34" s="38"/>
+      <c r="X37" s="38"/>
+      <c r="Y37" s="38"/>
+      <c r="Z37" s="38"/>
+      <c r="AA37" s="38"/>
+      <c r="AB37" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="98">
-    <mergeCell ref="W34:AB34"/>
-    <mergeCell ref="M34:P34"/>
-    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="W37:AB37"/>
+    <mergeCell ref="M37:P37"/>
+    <mergeCell ref="A37:F37"/>
     <mergeCell ref="A26:AB26"/>
     <mergeCell ref="AA27:AB27"/>
     <mergeCell ref="U27:Y27"/>
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="S32:T32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="S30:T30"/>
+    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I30:J30"/>
     <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="Q27:R27"/>
     <mergeCell ref="M5:U7"/>
     <mergeCell ref="M2:U4"/>
     <mergeCell ref="W7:AB7"/>
@@ -2331,8 +2413,6 @@
     <mergeCell ref="AA17:AB17"/>
     <mergeCell ref="AA15:AB15"/>
     <mergeCell ref="AA18:AB18"/>
-    <mergeCell ref="L10:P10"/>
-    <mergeCell ref="Q10:U10"/>
     <mergeCell ref="V10:Z10"/>
     <mergeCell ref="V11:V12"/>
     <mergeCell ref="Q25:U25"/>
@@ -2343,15 +2423,13 @@
     <mergeCell ref="V21:V22"/>
     <mergeCell ref="V23:V24"/>
     <mergeCell ref="V13:V14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="G15:G16"/>
     <mergeCell ref="G17:G18"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="G21:G22"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="L10:P10"/>
+    <mergeCell ref="Q10:U10"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q35:R35"/>
     <mergeCell ref="A9:AB9"/>
     <mergeCell ref="AA19:AB19"/>
     <mergeCell ref="AA20:AB20"/>
@@ -2364,6 +2442,8 @@
     <mergeCell ref="AA11:AB11"/>
     <mergeCell ref="AA12:AB12"/>
     <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G15:G16"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.22" right="0" top="0" bottom="0" header="0" footer="0.01"/>

</xml_diff>